<commit_message>
Création des profils : Évènement, Professionnel et Transport 24fe4b580b5bc70180e3d40bae36780e5d5864dd
</commit_message>
<xml_diff>
--- a/298-Ajout-de-l'évènement/ig/StructureDefinition-tddui-comment.xlsx
+++ b/298-Ajout-de-l'évènement/ig/StructureDefinition-tddui-comment.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-09-10T07:50:24+00:00</t>
+    <t>2025-09-10T10:00:26+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -81,7 +81,7 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Commentaire relatif au séjour.</t>
+    <t>Commentaire relatif au séjour et aux évènements.</t>
   </si>
   <si>
     <t>Purpose</t>

</xml_diff>